<commit_message>
Adding units for TC and TN
</commit_message>
<xml_diff>
--- a/data/metadata/water_chemistry_units.xlsx
+++ b/data/metadata/water_chemistry_units.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samstruthers/Documents/fork_yeah/CPF_reservoir_study_data/data/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samstruthers/Documents/fork_yeah/poudre_data_pub/CLP_waterchem_data/data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01749D43-37CE-F041-933A-1BF723609AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D7C9BA-50A0-7D44-A55A-9C79C4026CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>Parameters</t>
   </si>
@@ -583,6 +583,18 @@
   </si>
   <si>
     <t>SO4</t>
+  </si>
+  <si>
+    <t>TC (mg/L)</t>
+  </si>
+  <si>
+    <t>TN (mg/L)</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>TN</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1172,7 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>94456</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>34925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="65" cy="172227"/>
@@ -1215,9 +1227,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1255,7 +1267,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1361,7 +1373,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1503,7 +1515,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1511,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1581,208 +1593,236 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
         <v>27</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>